<commit_message>
roles doc team order update
</commit_message>
<xml_diff>
--- a/command-development-java/docs/team.xlsx
+++ b/command-development-java/docs/team.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\GeekBrains\command-development-java\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13ABDA36-C16B-4C6A-BEA5-33E433720E15}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FE7267-E7AD-4CA7-B593-8E8976B5C2FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D4D05BE9-CF8B-46CA-B3C8-E9FC8CC02F1F}"/>
   </bookViews>
@@ -438,7 +438,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,28 +467,28 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">

</xml_diff>